<commit_message>
Add tutorials for condition monitoring application.
</commit_message>
<xml_diff>
--- a/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/Test conditions.xlsx
+++ b/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/Test conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centralesupelec-my.sharepoint.com/personal/zhiguo_zeng_centralesupelec_fr/Documents/Code/Python/digital_twin_robot/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{764CB2E5-6CBA-48FE-848B-1DBDC1F1FC46}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D5B3398-9B9D-4246-997C-CBCAC9A99FBF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Test id</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Robot not moving.</t>
+  </si>
+  <si>
+    <t>20240321_122650</t>
+  </si>
+  <si>
+    <t>Try to move to pick up an item from second floor of a shelf. But failed.</t>
   </si>
 </sst>
 </file>
@@ -381,16 +387,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,6 +455,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create demo for data challenge.
</commit_message>
<xml_diff>
--- a/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/Test conditions.xlsx
+++ b/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/Test conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://centralesupelec-my.sharepoint.com/personal/zhiguo_zeng_centralesupelec_fr/Documents/Code/Python/digital_twin_robot/robot_digital_twin/condition_monitoring_matlab_ros/matlab_application/collected_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBDABE11-6EED-4BA3-8E55-F1208B668B34}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="11_F25DC773A252ABDACC1048B9511F42AE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D3F1547-6440-4310-A6A8-9A9741556532}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>Test id</t>
   </si>
@@ -133,16 +133,124 @@
   </si>
   <si>
     <t>Move motor 6 -&gt; motor 1 sequentially.</t>
+  </si>
+  <si>
+    <t>20240524_094684</t>
+  </si>
+  <si>
+    <t>20240524_094877</t>
+  </si>
+  <si>
+    <t>20240524_100052</t>
+  </si>
+  <si>
+    <t>Turning motor 1</t>
+  </si>
+  <si>
+    <t>Turning motor 2</t>
+  </si>
+  <si>
+    <t>20240524_101062</t>
+  </si>
+  <si>
+    <t>Turning motor 3</t>
+  </si>
+  <si>
+    <t>Turning motor 4</t>
+  </si>
+  <si>
+    <t>Turning motor 5</t>
+  </si>
+  <si>
+    <t>20240524_101487</t>
+  </si>
+  <si>
+    <t>20240524_102066</t>
+  </si>
+  <si>
+    <t>20240524_102736</t>
+  </si>
+  <si>
+    <t>20240524_103973</t>
+  </si>
+  <si>
+    <t>20240524_104453</t>
+  </si>
+  <si>
+    <t>20240524_102301</t>
+  </si>
+  <si>
+    <t>20240524_104923</t>
+  </si>
+  <si>
+    <t>20240524_105370</t>
+  </si>
+  <si>
+    <t>20240524_105836</t>
+  </si>
+  <si>
+    <t>20240524_110994</t>
+  </si>
+  <si>
+    <t>Perform motor 1 fail</t>
+  </si>
+  <si>
+    <t>Perform motor 2 fail</t>
+  </si>
+  <si>
+    <t>Perform motor 3 fail</t>
+  </si>
+  <si>
+    <t>Perform motor 4 fail</t>
+  </si>
+  <si>
+    <t>Perform motor 5 fail</t>
+  </si>
+  <si>
+    <t>Perform motor 321654 fail</t>
+  </si>
+  <si>
+    <t>20240527_094865</t>
+  </si>
+  <si>
+    <t>Transfer goods</t>
+  </si>
+  <si>
+    <t>20240527_100759</t>
+  </si>
+  <si>
+    <t>20240527_101627</t>
+  </si>
+  <si>
+    <t>20240527_102436</t>
+  </si>
+  <si>
+    <t>20240527_102919</t>
+  </si>
+  <si>
+    <t>20240527_103311</t>
+  </si>
+  <si>
+    <t>20240527_103690</t>
+  </si>
+  <si>
+    <t>20240527_104247</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -450,20 +558,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -497,7 +605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -505,7 +613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,7 +621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -521,7 +629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -529,7 +637,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -537,7 +645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -545,7 +653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -553,7 +661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -561,7 +669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -587,7 +695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -598,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -609,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -635,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -643,7 +751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -651,7 +759,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -659,7 +767,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -667,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -675,7 +783,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -683,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -694,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -702,7 +810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -713,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -724,7 +832,329 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>